<commit_message>
fix full store type, qsr template, etc
</commit_message>
<xml_diff>
--- a/Projects/CCBZA/Data/Template_QSR.xlsx
+++ b/Projects/CCBZA/Data/Template_QSR.xlsx
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$13</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">Availability!$A$1:$S$13</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$S$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -405,7 +406,7 @@
     <t xml:space="preserve">SSD</t>
   </si>
   <si>
-    <t xml:space="preserve">Category</t>
+    <t xml:space="preserve">category</t>
   </si>
 </sst>
 </file>
@@ -715,19 +716,19 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.1813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,19 +1098,19 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="113.218604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="66.6976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="116.66511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="68.7906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1189,21 +1190,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="76.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="56.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="78.5116279069767"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,20 +1364,20 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="116.293023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="119.739534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,31 +1718,31 @@
   </sheetPr>
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="36.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.98139534883721"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="37.1627906976744"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,29 +2354,29 @@
   </sheetPr>
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,9 +2554,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.246511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>